<commit_message>
Add not personal model
</commit_message>
<xml_diff>
--- a/icarbonx_data/train&test/y_test.xlsx
+++ b/icarbonx_data/train&test/y_test.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B541"/>
+  <dimension ref="A1:B545"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -382,7 +382,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>121.275</v>
+        <v>48.1333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -390,7 +390,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>49.5</v>
+        <v>36.25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>38.75</v>
+        <v>27.25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -406,7 +406,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>34.5916666666666</v>
+        <v>85.9166666666666</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>13.25</v>
+        <v>67.9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>16.9666666666666</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -446,7 +446,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>88.3833333333333</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63.5666666666666</v>
+        <v>44.875</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -470,7 +470,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>22.0833333333333</v>
+        <v>31.2333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -478,7 +478,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>39.375</v>
+        <v>11.1214285714285</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -486,7 +486,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>27.25</v>
+        <v>7.375</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -494,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>20.6416666666666</v>
+        <v>14.8928571428571</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -502,7 +502,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>22.75</v>
+        <v>12.625</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -510,7 +510,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>47</v>
+        <v>25.875</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -518,7 +518,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>34.875</v>
+        <v>48.725</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -526,7 +526,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>23.8926470588235</v>
+        <v>6.79166666666666</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -534,7 +534,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>41.2</v>
+        <v>33.5703125</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -542,7 +542,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>28.75</v>
+        <v>15.875</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -550,7 +550,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>23.0833333333333</v>
+        <v>28.125</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -558,7 +558,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>39.1833333333333</v>
+        <v>17.2333333333333</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -566,7 +566,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>40.75</v>
+        <v>28.75</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -574,7 +574,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>71.60833333333331</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -582,7 +582,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>53.125</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -590,7 +590,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12.7053571428571</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -598,7 +598,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>44.25</v>
+        <v>39.875</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -606,7 +606,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>73.82692307692299</v>
+        <v>37.75</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -614,7 +614,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>33.2083333333333</v>
+        <v>52.75</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -622,7 +622,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>14.9318181818181</v>
+        <v>69.025</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -630,7 +630,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>58.375</v>
+        <v>35.7583333333333</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -638,7 +638,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>48.8333333333333</v>
+        <v>40.75</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -646,7 +646,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>104.875</v>
+        <v>97.6166666666666</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -654,7 +654,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>32.8333333333333</v>
+        <v>24.8916666666666</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -662,7 +662,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>29.0166666666666</v>
+        <v>6.13636363636363</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -670,7 +670,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>39.8916666666666</v>
+        <v>17.5238095238095</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -678,7 +678,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>11.9166666666666</v>
+        <v>6.18452380952381</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -686,7 +686,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>11.6375</v>
+        <v>17.8375</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -694,7 +694,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>11.7666666666666</v>
+        <v>5.23333333333333</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -702,7 +702,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>85.125</v>
+        <v>63.2916666666666</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -710,7 +710,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>54.75</v>
+        <v>26.6416666666666</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -718,7 +718,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>27.67</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -726,7 +726,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>21.175</v>
+        <v>20.5869565217391</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -734,7 +734,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>14.25</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -742,7 +742,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>11.96875</v>
+        <v>37.025</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -750,7 +750,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>23.6875</v>
+        <v>56.5916666666666</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -758,7 +758,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>15.3863636363636</v>
+        <v>14.1458333333333</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -766,7 +766,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>16.375</v>
+        <v>48.825</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -774,7 +774,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -782,7 +782,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>21.5666666666666</v>
+        <v>153.375</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -790,7 +790,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>72.4083333333333</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -798,7 +798,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>25.125</v>
+        <v>26.875</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -806,7 +806,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>18.2053571428571</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -814,7 +814,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>25.95</v>
+        <v>34.875</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -830,7 +830,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>20.75</v>
+        <v>33.6833333333333</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -838,7 +838,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>31.375</v>
+        <v>71.5714285714285</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -846,7 +846,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>48.1333333333333</v>
+        <v>29.25</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -854,7 +854,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>14.75</v>
+        <v>13.175</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -862,7 +862,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>10.4567307692307</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -870,7 +870,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>11.2291666666666</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -878,7 +878,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>6.515625</v>
+        <v>22.05</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -886,7 +886,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>6.54347826086956</v>
+        <v>18.5583333333333</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -894,7 +894,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>66</v>
+        <v>42.25</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -902,7 +902,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>33.5703125</v>
+        <v>16.15625</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -910,7 +910,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>15.75</v>
+        <v>11.9166666666666</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -918,7 +918,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>66.25</v>
+        <v>13.3958333333333</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -926,7 +926,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>35</v>
+        <v>10.8666666666666</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -934,7 +934,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>37.625</v>
+        <v>34.5916666666666</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -942,7 +942,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>79</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -950,7 +950,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>15.7222222222222</v>
+        <v>14.2166666666666</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -958,7 +958,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>24.3806818181818</v>
+        <v>32.8083333333333</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -966,7 +966,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>24.7916666666666</v>
+        <v>10.95</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -974,7 +974,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>28.1805555555555</v>
+        <v>89.375</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -982,7 +982,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>42.55</v>
+        <v>13.8572916666666</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -990,7 +990,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>52.875</v>
+        <v>9.17708333333333</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -998,7 +998,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>85.9166666666666</v>
+        <v>15.3863636363636</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>93.625</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1014,7 +1014,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>44</v>
+        <v>13.0833333333333</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>15.125</v>
+        <v>61.75</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1030,7 +1030,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>18.0555555555555</v>
+        <v>64.5416666666666</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1038,7 +1038,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>4.75</v>
+        <v>24.3806818181818</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>57.125</v>
+        <v>29.1007575757575</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1062,7 +1062,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>45.4375</v>
+        <v>41.75</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>52.25</v>
+        <v>35.6323529411764</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>10.05</v>
+        <v>78.3666666666666</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1086,7 +1086,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>7.85238095238095</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1094,7 +1094,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>37.625</v>
+        <v>27.9666666666666</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1102,7 +1102,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>18.88</v>
+        <v>47.625</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>20.5869565217391</v>
+        <v>34.875</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>40.375</v>
+        <v>61.6666666666666</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>28.75</v>
+        <v>11.3791666666666</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1134,7 +1134,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>48.25</v>
+        <v>12.0380952380952</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1142,7 +1142,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>33.875</v>
+        <v>52.75</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1150,7 +1150,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>72.75</v>
+        <v>46.1166666666666</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>34.4375</v>
+        <v>38.375</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>37.875</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>31.6583333333333</v>
+        <v>38.75</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1182,7 +1182,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>6.18452380952381</v>
+        <v>28.6622549019607</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1190,7 +1190,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>48.0833333333333</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1198,7 +1198,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>17.85</v>
+        <v>35.625</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1206,7 +1206,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>33.6833333333333</v>
+        <v>33.1333333333333</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1214,7 +1214,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>20.2986111111111</v>
+        <v>22.125</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1222,7 +1222,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>81.325</v>
+        <v>57.125</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1230,7 +1230,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>26.875</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1238,7 +1238,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>25.875</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1246,7 +1246,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>5.38888888888888</v>
+        <v>14.3815789473684</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1254,7 +1254,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>8.64583333333333</v>
+        <v>64.5833333333333</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1278,7 +1278,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>5.77272727272727</v>
+        <v>23.6416666666666</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1286,7 +1286,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>61.8661764705882</v>
+        <v>13.8214285714285</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1294,7 +1294,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>17.375</v>
+        <v>44.25</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1302,7 +1302,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>14.8875</v>
+        <v>18.625</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1310,7 +1310,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>40.875</v>
+        <v>34.375</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1318,7 +1318,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>14.25</v>
+        <v>39.9666666666666</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1326,7 +1326,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>18.75</v>
+        <v>22.0833333333333</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1334,7 +1334,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>11</v>
+        <v>20.875</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1342,7 +1342,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>9.93125</v>
+        <v>85.125</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1350,7 +1350,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>37.75</v>
+        <v>60.725</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1358,7 +1358,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>20.25</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1366,7 +1366,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>35.5</v>
+        <v>7.16666666666666</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1374,7 +1374,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>77.75</v>
+        <v>49.1916666666666</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1382,7 +1382,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>49.1916666666666</v>
+        <v>31.6583333333333</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1390,7 +1390,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>14.875</v>
+        <v>26.1666666666666</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1398,7 +1398,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>64.5833333333333</v>
+        <v>41.2</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1406,7 +1406,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>49.875</v>
+        <v>25.25</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1414,7 +1414,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>35.7583333333333</v>
+        <v>34.4375</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1422,7 +1422,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>35.6833333333333</v>
+        <v>32.65</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1430,7 +1430,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>5.90384615384615</v>
+        <v>63.25</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1438,7 +1438,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>36.5333333333333</v>
+        <v>16.2666666666666</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1446,7 +1446,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>178.5</v>
+        <v>22.125</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1454,7 +1454,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>32.9666666666666</v>
+        <v>19.125</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1462,7 +1462,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>23.8958333333333</v>
+        <v>30.25</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1470,7 +1470,7 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>7.57142857142857</v>
+        <v>38.875</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1478,7 +1478,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>31.2333333333333</v>
+        <v>11.96875</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1486,7 +1486,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>6.13636363636363</v>
+        <v>30.1388888888888</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1494,7 +1494,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>8.928623188405791</v>
+        <v>27.2416666666666</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1502,7 +1502,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>27.5</v>
+        <v>26.375</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1510,7 +1510,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>18.5583333333333</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1518,7 +1518,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>71.4083333333333</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1526,7 +1526,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>11</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1534,7 +1534,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>23.625</v>
+        <v>18</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1542,7 +1542,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>5.5</v>
+        <v>82.3916666666666</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1550,7 +1550,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>24.3166666666666</v>
+        <v>48.7916666666666</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1558,7 +1558,7 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>42.5484848484848</v>
+        <v>14.0666666666666</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1566,7 +1566,7 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>62.75</v>
+        <v>31.95</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1574,7 +1574,7 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>32.25</v>
+        <v>17.625</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1582,7 +1582,7 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>16.15625</v>
+        <v>10.6875</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1590,7 +1590,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>35.625</v>
+        <v>47.875</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1598,7 +1598,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>37.75</v>
+        <v>82.125</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1606,7 +1606,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>69.625</v>
+        <v>34.375</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1614,7 +1614,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>39.1682692307692</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1622,7 +1622,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>21.5384615384615</v>
+        <v>19.875</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1630,7 +1630,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>47.625</v>
+        <v>18.525</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1638,7 +1638,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>73.25</v>
+        <v>54.7948717948717</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1646,7 +1646,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>38.25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1654,7 +1654,7 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>41</v>
+        <v>30.875</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1662,7 +1662,7 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>54.7948717948717</v>
+        <v>44.625</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1670,7 +1670,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>43.3916666666666</v>
+        <v>53</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1678,7 +1678,7 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>100.041666666666</v>
+        <v>63.5666666666666</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1686,7 +1686,7 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>42.9166666666666</v>
+        <v>45.8333333333333</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1694,7 +1694,7 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>53.2666666666666</v>
+        <v>23.5845238095238</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1702,7 +1702,7 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>14.2293233082706</v>
+        <v>23.625</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1710,7 +1710,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>27.625</v>
+        <v>18.88</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1718,7 +1718,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>33.1333333333333</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1726,7 +1726,7 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>11.15</v>
+        <v>21.4666666666666</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1734,7 +1734,7 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>54.8666666666666</v>
+        <v>49.875</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1742,7 +1742,7 @@
         <v>170</v>
       </c>
       <c r="B172">
-        <v>17.8083333333333</v>
+        <v>9</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1750,7 +1750,7 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>65.625</v>
+        <v>11.2291666666666</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1758,7 +1758,7 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>52.875</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1766,7 +1766,7 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>37.375</v>
+        <v>41.875</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1774,7 +1774,7 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>5.23333333333333</v>
+        <v>41</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1782,7 +1782,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>32</v>
+        <v>19.6083333333333</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1790,7 +1790,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>16.2666666666666</v>
+        <v>42.55</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1798,7 +1798,7 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>10.8916666666666</v>
+        <v>43.87</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1806,7 +1806,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>47.5166666666666</v>
+        <v>20.2986111111111</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1814,7 +1814,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>61.925</v>
+        <v>19.025</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1822,7 +1822,7 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>107.75</v>
+        <v>41.6944444444444</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1830,7 +1830,7 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>27.45</v>
+        <v>19.375</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1838,7 +1838,7 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>50</v>
+        <v>6.54347826086956</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1846,7 +1846,7 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>13.8214285714285</v>
+        <v>13.8653846153846</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1854,7 +1854,7 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>35.625</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1862,7 +1862,7 @@
         <v>185</v>
       </c>
       <c r="B187">
-        <v>31.25</v>
+        <v>51.625</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1870,7 +1870,7 @@
         <v>186</v>
       </c>
       <c r="B188">
-        <v>25.2656862745098</v>
+        <v>21.5666666666666</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1878,7 +1878,7 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>14.3815789473684</v>
+        <v>25.625</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1886,7 +1886,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>30.1388888888888</v>
+        <v>18.1125</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1894,7 +1894,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>22.6590909090909</v>
+        <v>28.4916666666666</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1902,7 +1902,7 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>34.375</v>
+        <v>5.0703125</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1910,7 +1910,7 @@
         <v>191</v>
       </c>
       <c r="B193">
-        <v>18.1125</v>
+        <v>23.8958333333333</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1918,7 +1918,7 @@
         <v>192</v>
       </c>
       <c r="B194">
-        <v>15.2458333333333</v>
+        <v>66.625</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1926,7 +1926,7 @@
         <v>193</v>
       </c>
       <c r="B195">
-        <v>29.25</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1934,7 +1934,7 @@
         <v>194</v>
       </c>
       <c r="B196">
-        <v>18.25</v>
+        <v>12.07</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1942,7 +1942,7 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>61.1833333333333</v>
+        <v>30.3833333333333</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1950,7 +1950,7 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>97.6166666666666</v>
+        <v>61.125</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1958,7 +1958,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>7.97727272727272</v>
+        <v>59.125</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1966,7 +1966,7 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>32.25</v>
+        <v>81.325</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1974,7 +1974,7 @@
         <v>199</v>
       </c>
       <c r="B201">
-        <v>23.25</v>
+        <v>18.2053571428571</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -1982,7 +1982,7 @@
         <v>200</v>
       </c>
       <c r="B202">
-        <v>29.875</v>
+        <v>7.85238095238095</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -1990,7 +1990,7 @@
         <v>201</v>
       </c>
       <c r="B203">
-        <v>5.14285714285714</v>
+        <v>27.45</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -1998,7 +1998,7 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>13.375</v>
+        <v>8.94117647058823</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2006,7 +2006,7 @@
         <v>203</v>
       </c>
       <c r="B205">
-        <v>14.2857142857142</v>
+        <v>16.7416666666666</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2014,7 +2014,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>22.05</v>
+        <v>60.6083333333333</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2022,7 +2022,7 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>8.94117647058823</v>
+        <v>36.2410256410256</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2030,7 +2030,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>16.7416666666666</v>
+        <v>24.4666666666666</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2038,7 +2038,7 @@
         <v>207</v>
       </c>
       <c r="B209">
-        <v>60.6083333333333</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2046,7 +2046,7 @@
         <v>208</v>
       </c>
       <c r="B210">
-        <v>78.125</v>
+        <v>5.3875</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2054,7 +2054,7 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>47.875</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2062,7 +2062,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>17.625</v>
+        <v>39.8916666666666</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2070,7 +2070,7 @@
         <v>211</v>
       </c>
       <c r="B213">
-        <v>52.75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2078,7 +2078,7 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>5.75</v>
+        <v>9.93125</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2086,7 +2086,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>5.75</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2094,7 +2094,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>15.7916666666666</v>
+        <v>80.875</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2102,7 +2102,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>9.513888888888889</v>
+        <v>66.25</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2110,7 +2110,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>19.1145833333333</v>
+        <v>4.87447916666666</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2118,7 +2118,7 @@
         <v>217</v>
       </c>
       <c r="B219">
-        <v>13.125</v>
+        <v>25.125</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2126,7 +2126,7 @@
         <v>218</v>
       </c>
       <c r="B220">
-        <v>65.625</v>
+        <v>8.65625</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2134,7 +2134,7 @@
         <v>219</v>
       </c>
       <c r="B221">
-        <v>15.5</v>
+        <v>30.025</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2142,7 +2142,7 @@
         <v>220</v>
       </c>
       <c r="B222">
-        <v>39.675</v>
+        <v>37.875</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2150,7 +2150,7 @@
         <v>221</v>
       </c>
       <c r="B223">
-        <v>8.65625</v>
+        <v>49.3333333333333</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2158,7 +2158,7 @@
         <v>222</v>
       </c>
       <c r="B224">
-        <v>17.625</v>
+        <v>58.375</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2166,7 +2166,7 @@
         <v>223</v>
       </c>
       <c r="B225">
-        <v>54.2416666666666</v>
+        <v>42.7833333333333</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2174,7 +2174,7 @@
         <v>224</v>
       </c>
       <c r="B226">
-        <v>60.875</v>
+        <v>41.95</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2182,7 +2182,7 @@
         <v>225</v>
       </c>
       <c r="B227">
-        <v>10.5833333333333</v>
+        <v>40.875</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2190,7 +2190,7 @@
         <v>226</v>
       </c>
       <c r="B228">
-        <v>32.9</v>
+        <v>16.125</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2198,7 +2198,7 @@
         <v>227</v>
       </c>
       <c r="B229">
-        <v>42.975</v>
+        <v>35</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2206,7 +2206,7 @@
         <v>228</v>
       </c>
       <c r="B230">
-        <v>84.375</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2214,7 +2214,7 @@
         <v>229</v>
       </c>
       <c r="B231">
-        <v>16.125</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2222,7 +2222,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>32.625</v>
+        <v>61.9</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2230,7 +2230,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>16</v>
+        <v>92.375</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2238,7 +2238,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>23.6416666666666</v>
+        <v>45.25</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2246,7 +2246,7 @@
         <v>233</v>
       </c>
       <c r="B235">
-        <v>13.125</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2254,7 +2254,7 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>10.95</v>
+        <v>27.25</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2262,7 +2262,7 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>17.5</v>
+        <v>5.31666666666666</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2270,7 +2270,7 @@
         <v>236</v>
       </c>
       <c r="B238">
-        <v>17</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2278,7 +2278,7 @@
         <v>237</v>
       </c>
       <c r="B239">
-        <v>13.8653846153846</v>
+        <v>4.38333333333333</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2286,7 +2286,7 @@
         <v>238</v>
       </c>
       <c r="B240">
-        <v>48.5</v>
+        <v>37.8666666666666</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2294,7 +2294,7 @@
         <v>239</v>
       </c>
       <c r="B241">
-        <v>7.875</v>
+        <v>52.875</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2302,7 +2302,7 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>56.8666666666666</v>
+        <v>14.9318181818181</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2310,7 +2310,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>15.7833333333333</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2318,7 +2318,7 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>1.8</v>
+        <v>93.625</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2326,7 +2326,7 @@
         <v>243</v>
       </c>
       <c r="B245">
-        <v>44.875</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2334,7 +2334,7 @@
         <v>244</v>
       </c>
       <c r="B246">
-        <v>12</v>
+        <v>18.4166666666666</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2342,7 +2342,7 @@
         <v>245</v>
       </c>
       <c r="B247">
-        <v>28.4</v>
+        <v>28.75</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2350,7 +2350,7 @@
         <v>246</v>
       </c>
       <c r="B248">
-        <v>28.55</v>
+        <v>19.5416666666666</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2358,7 +2358,7 @@
         <v>247</v>
       </c>
       <c r="B249">
-        <v>18.7888888888888</v>
+        <v>13.4166666666666</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2366,7 +2366,7 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>69.375</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2374,7 +2374,7 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>14.625</v>
+        <v>35.625</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2382,7 +2382,7 @@
         <v>250</v>
       </c>
       <c r="B252">
-        <v>19.375</v>
+        <v>37.25</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2390,7 +2390,7 @@
         <v>251</v>
       </c>
       <c r="B253">
-        <v>14.0666666666666</v>
+        <v>27.625</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2398,7 +2398,7 @@
         <v>252</v>
       </c>
       <c r="B254">
-        <v>37.9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2406,7 +2406,7 @@
         <v>253</v>
       </c>
       <c r="B255">
-        <v>68.2</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2414,7 +2414,7 @@
         <v>254</v>
       </c>
       <c r="B256">
-        <v>8.93928571428571</v>
+        <v>14.875</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2422,7 +2422,7 @@
         <v>255</v>
       </c>
       <c r="B257">
-        <v>27.625</v>
+        <v>13.375</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2430,7 +2430,7 @@
         <v>256</v>
       </c>
       <c r="B258">
-        <v>33.0166666666666</v>
+        <v>12.8638888888888</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2438,7 +2438,7 @@
         <v>257</v>
       </c>
       <c r="B259">
-        <v>38.875</v>
+        <v>34.9342105263157</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2446,7 +2446,7 @@
         <v>258</v>
       </c>
       <c r="B260">
-        <v>12.8638888888888</v>
+        <v>49.125</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2454,7 +2454,7 @@
         <v>259</v>
       </c>
       <c r="B261">
-        <v>61.85</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2462,7 +2462,7 @@
         <v>260</v>
       </c>
       <c r="B262">
-        <v>49.125</v>
+        <v>77</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2470,7 +2470,7 @@
         <v>261</v>
       </c>
       <c r="B263">
-        <v>23.5</v>
+        <v>33.4166666666666</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2478,7 +2478,7 @@
         <v>262</v>
       </c>
       <c r="B264">
-        <v>56.75</v>
+        <v>45.25</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2486,7 +2486,7 @@
         <v>263</v>
       </c>
       <c r="B265">
-        <v>52.7083333333333</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2494,7 +2494,7 @@
         <v>264</v>
       </c>
       <c r="B266">
-        <v>25.4868421052631</v>
+        <v>36.625</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2502,7 +2502,7 @@
         <v>265</v>
       </c>
       <c r="B267">
-        <v>27.2884615384615</v>
+        <v>39.625</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2510,7 +2510,7 @@
         <v>266</v>
       </c>
       <c r="B268">
-        <v>17.9722222222222</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2518,7 +2518,7 @@
         <v>267</v>
       </c>
       <c r="B269">
-        <v>23.125</v>
+        <v>17.9722222222222</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2526,7 +2526,7 @@
         <v>268</v>
       </c>
       <c r="B270">
-        <v>24.125</v>
+        <v>27.2884615384615</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2534,7 +2534,7 @@
         <v>269</v>
       </c>
       <c r="B271">
-        <v>19.8809523809523</v>
+        <v>25.4868421052631</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2542,7 +2542,7 @@
         <v>270</v>
       </c>
       <c r="B272">
-        <v>19.525</v>
+        <v>23.125</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2550,7 +2550,7 @@
         <v>271</v>
       </c>
       <c r="B273">
-        <v>17.925</v>
+        <v>24.125</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2558,7 +2558,7 @@
         <v>272</v>
       </c>
       <c r="B274">
-        <v>23.25</v>
+        <v>4.04545454545454</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2566,7 +2566,7 @@
         <v>273</v>
       </c>
       <c r="B275">
-        <v>59.125</v>
+        <v>17.925</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -2574,7 +2574,7 @@
         <v>274</v>
       </c>
       <c r="B276">
-        <v>35.6323529411764</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -2582,7 +2582,7 @@
         <v>275</v>
       </c>
       <c r="B277">
-        <v>39.9</v>
+        <v>48.05</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -2590,7 +2590,7 @@
         <v>276</v>
       </c>
       <c r="B278">
-        <v>38.125</v>
+        <v>30.875</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2598,7 +2598,7 @@
         <v>277</v>
       </c>
       <c r="B279">
-        <v>12.375</v>
+        <v>29.625</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2606,7 +2606,7 @@
         <v>278</v>
       </c>
       <c r="B280">
-        <v>33.125</v>
+        <v>30.2833333333333</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2614,7 +2614,7 @@
         <v>279</v>
       </c>
       <c r="B281">
-        <v>19.5</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2622,7 +2622,7 @@
         <v>280</v>
       </c>
       <c r="B282">
-        <v>18.75</v>
+        <v>11.9615384615384</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2630,7 +2630,7 @@
         <v>281</v>
       </c>
       <c r="B283">
-        <v>39.6333333333333</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2638,7 +2638,7 @@
         <v>282</v>
       </c>
       <c r="B284">
-        <v>34.75</v>
+        <v>3.72727272727272</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2646,7 +2646,7 @@
         <v>283</v>
       </c>
       <c r="B285">
-        <v>37.25</v>
+        <v>13.4375</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2654,7 +2654,7 @@
         <v>284</v>
       </c>
       <c r="B286">
-        <v>22.125</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2662,7 +2662,7 @@
         <v>285</v>
       </c>
       <c r="B287">
-        <v>21.75</v>
+        <v>7.91666666666666</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2670,7 +2670,7 @@
         <v>286</v>
       </c>
       <c r="B288">
-        <v>18.375</v>
+        <v>12.175</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2678,7 +2678,7 @@
         <v>287</v>
       </c>
       <c r="B289">
-        <v>12.1875</v>
+        <v>26.375</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2686,7 +2686,7 @@
         <v>288</v>
       </c>
       <c r="B290">
-        <v>37.75</v>
+        <v>18.375</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -2694,7 +2694,7 @@
         <v>289</v>
       </c>
       <c r="B291">
-        <v>51.475</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2702,7 +2702,7 @@
         <v>290</v>
       </c>
       <c r="B292">
-        <v>17.8</v>
+        <v>27.6375</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -2710,7 +2710,7 @@
         <v>291</v>
       </c>
       <c r="B293">
-        <v>6.125</v>
+        <v>22.0071428571428</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2718,7 +2718,7 @@
         <v>292</v>
       </c>
       <c r="B294">
-        <v>12</v>
+        <v>18.625</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2726,7 +2726,7 @@
         <v>293</v>
       </c>
       <c r="B295">
-        <v>18.5</v>
+        <v>27.825</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2734,7 +2734,7 @@
         <v>294</v>
       </c>
       <c r="B296">
-        <v>33.3214285714285</v>
+        <v>30.5833333333333</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2742,7 +2742,7 @@
         <v>295</v>
       </c>
       <c r="B297">
-        <v>37.0416666666666</v>
+        <v>34.625</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2750,7 +2750,7 @@
         <v>296</v>
       </c>
       <c r="B298">
-        <v>18.7375</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2758,7 +2758,7 @@
         <v>297</v>
       </c>
       <c r="B299">
-        <v>23.25</v>
+        <v>35.125</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2766,7 +2766,7 @@
         <v>298</v>
       </c>
       <c r="B300">
-        <v>26.7138888888888</v>
+        <v>30.2916666666666</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2774,7 +2774,7 @@
         <v>299</v>
       </c>
       <c r="B301">
-        <v>17.875</v>
+        <v>27.375</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2782,7 +2782,7 @@
         <v>300</v>
       </c>
       <c r="B302">
-        <v>18</v>
+        <v>25.0166666666666</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2790,7 +2790,7 @@
         <v>301</v>
       </c>
       <c r="B303">
-        <v>13.15625</v>
+        <v>19.5238095238095</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2798,7 +2798,7 @@
         <v>302</v>
       </c>
       <c r="B304">
-        <v>9.17708333333333</v>
+        <v>17.875</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2806,7 +2806,7 @@
         <v>303</v>
       </c>
       <c r="B305">
-        <v>12.93125</v>
+        <v>18</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2814,7 +2814,7 @@
         <v>304</v>
       </c>
       <c r="B306">
-        <v>11.1363636363636</v>
+        <v>13.15625</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2822,7 +2822,7 @@
         <v>305</v>
       </c>
       <c r="B307">
-        <v>10.5</v>
+        <v>14.4318181818181</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2830,7 +2830,7 @@
         <v>306</v>
       </c>
       <c r="B308">
-        <v>13.3958333333333</v>
+        <v>14.125</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2838,7 +2838,7 @@
         <v>307</v>
       </c>
       <c r="B309">
-        <v>14.25</v>
+        <v>16.9666666666666</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2846,7 +2846,7 @@
         <v>308</v>
       </c>
       <c r="B310">
-        <v>13.0083333333333</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2854,7 +2854,7 @@
         <v>309</v>
       </c>
       <c r="B311">
-        <v>6.75</v>
+        <v>37.1333333333333</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -2862,7 +2862,7 @@
         <v>310</v>
       </c>
       <c r="B312">
-        <v>13.2954545454545</v>
+        <v>32.7115384615384</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2870,7 +2870,7 @@
         <v>311</v>
       </c>
       <c r="B313">
-        <v>7.625</v>
+        <v>34.75</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2878,7 +2878,7 @@
         <v>312</v>
       </c>
       <c r="B314">
-        <v>9.09848484848485</v>
+        <v>37.225</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2886,7 +2886,7 @@
         <v>313</v>
       </c>
       <c r="B315">
-        <v>10.5</v>
+        <v>45.5333333333333</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2894,7 +2894,7 @@
         <v>314</v>
       </c>
       <c r="B316">
-        <v>13.8833333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2902,7 +2902,7 @@
         <v>315</v>
       </c>
       <c r="B317">
-        <v>17.9375</v>
+        <v>26.1166666666666</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2910,7 +2910,7 @@
         <v>316</v>
       </c>
       <c r="B318">
-        <v>21.1</v>
+        <v>9.09821428571428</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2918,7 +2918,7 @@
         <v>317</v>
       </c>
       <c r="B319">
-        <v>32.5</v>
+        <v>9.58333333333333</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2926,7 +2926,7 @@
         <v>318</v>
       </c>
       <c r="B320">
-        <v>26.7954545454545</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2934,7 +2934,7 @@
         <v>319</v>
       </c>
       <c r="B321">
-        <v>12.0333333333333</v>
+        <v>14.2583333333333</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2942,7 +2942,7 @@
         <v>320</v>
       </c>
       <c r="B322">
-        <v>20.625</v>
+        <v>27.125</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2950,7 +2950,7 @@
         <v>321</v>
       </c>
       <c r="B323">
-        <v>13.8863636363636</v>
+        <v>26.7166666666666</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2958,7 +2958,7 @@
         <v>322</v>
       </c>
       <c r="B324">
-        <v>17.375</v>
+        <v>29.6309523809523</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2966,7 +2966,7 @@
         <v>323</v>
       </c>
       <c r="B325">
-        <v>8.625</v>
+        <v>17.4875</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -2974,7 +2974,7 @@
         <v>324</v>
       </c>
       <c r="B326">
-        <v>12.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -2982,7 +2982,7 @@
         <v>325</v>
       </c>
       <c r="B327">
-        <v>10.7083333333333</v>
+        <v>21.0961538461538</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -2990,7 +2990,7 @@
         <v>326</v>
       </c>
       <c r="B328">
-        <v>8.63461538461538</v>
+        <v>26.5666666666666</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -2998,7 +2998,7 @@
         <v>327</v>
       </c>
       <c r="B329">
-        <v>16.1666666666666</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3006,7 +3006,7 @@
         <v>328</v>
       </c>
       <c r="B330">
-        <v>10.75</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3014,7 +3014,7 @@
         <v>329</v>
       </c>
       <c r="B331">
-        <v>15.25</v>
+        <v>20.40625</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3022,7 +3022,7 @@
         <v>330</v>
       </c>
       <c r="B332">
-        <v>33.25</v>
+        <v>27.67</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3030,7 +3030,7 @@
         <v>331</v>
       </c>
       <c r="B333">
-        <v>31.1916666666666</v>
+        <v>19.5916666666666</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3038,7 +3038,7 @@
         <v>332</v>
       </c>
       <c r="B334">
-        <v>37.25</v>
+        <v>26.7138888888888</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3046,7 +3046,7 @@
         <v>333</v>
       </c>
       <c r="B335">
-        <v>16.765625</v>
+        <v>29.7880952380952</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3054,7 +3054,7 @@
         <v>334</v>
       </c>
       <c r="B336">
-        <v>22.375</v>
+        <v>33.125</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3062,7 +3062,7 @@
         <v>335</v>
       </c>
       <c r="B337">
-        <v>14.7397435897435</v>
+        <v>31.1916666666666</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3070,7 +3070,7 @@
         <v>336</v>
       </c>
       <c r="B338">
-        <v>14.75</v>
+        <v>27</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3078,7 +3078,7 @@
         <v>337</v>
       </c>
       <c r="B339">
-        <v>21.8203125</v>
+        <v>17.375</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3086,7 +3086,7 @@
         <v>338</v>
       </c>
       <c r="B340">
-        <v>15.75</v>
+        <v>10.375</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3094,7 +3094,7 @@
         <v>339</v>
       </c>
       <c r="B341">
-        <v>14.125</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3102,7 +3102,7 @@
         <v>340</v>
       </c>
       <c r="B342">
-        <v>27.9666666666666</v>
+        <v>23.525</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3110,7 +3110,7 @@
         <v>341</v>
       </c>
       <c r="B343">
-        <v>33.625</v>
+        <v>11.046875</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3118,7 +3118,7 @@
         <v>342</v>
       </c>
       <c r="B344">
-        <v>25.125</v>
+        <v>6.38541666666666</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3126,7 +3126,7 @@
         <v>343</v>
       </c>
       <c r="B345">
-        <v>13.4375</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3134,7 +3134,7 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>10.3214285714285</v>
+        <v>8.21666666666666</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3142,7 +3142,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>12.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3150,7 +3150,7 @@
         <v>346</v>
       </c>
       <c r="B348">
-        <v>12.175</v>
+        <v>15.4375</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3158,7 +3158,7 @@
         <v>347</v>
       </c>
       <c r="B349">
-        <v>6.875</v>
+        <v>22.8898809523809</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3166,7 +3166,7 @@
         <v>348</v>
       </c>
       <c r="B350">
-        <v>13.1666666666666</v>
+        <v>18.625</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3174,7 +3174,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>7.68</v>
+        <v>11.1363636363636</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3182,7 +3182,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>11.0026923076923</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3190,7 +3190,7 @@
         <v>351</v>
       </c>
       <c r="B353">
-        <v>27.375</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3198,7 +3198,7 @@
         <v>352</v>
       </c>
       <c r="B354">
-        <v>27.75</v>
+        <v>13.0083333333333</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3206,7 +3206,7 @@
         <v>353</v>
       </c>
       <c r="B355">
-        <v>30.5833333333333</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3214,7 +3214,7 @@
         <v>354</v>
       </c>
       <c r="B356">
-        <v>34.625</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3222,7 +3222,7 @@
         <v>355</v>
       </c>
       <c r="B357">
-        <v>35.125</v>
+        <v>19.875</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3230,7 +3230,7 @@
         <v>356</v>
       </c>
       <c r="B358">
-        <v>24.5</v>
+        <v>13.2954545454545</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3238,7 +3238,7 @@
         <v>357</v>
       </c>
       <c r="B359">
-        <v>30.2916666666666</v>
+        <v>24.375</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3246,7 +3246,7 @@
         <v>358</v>
       </c>
       <c r="B360">
-        <v>27.825</v>
+        <v>23.6666666666666</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3254,7 +3254,7 @@
         <v>359</v>
       </c>
       <c r="B361">
-        <v>25.0166666666666</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3262,7 +3262,7 @@
         <v>360</v>
       </c>
       <c r="B362">
-        <v>19.5238095238095</v>
+        <v>9.625</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3270,7 +3270,7 @@
         <v>361</v>
       </c>
       <c r="B363">
-        <v>27.5</v>
+        <v>8.1875</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3278,7 +3278,7 @@
         <v>362</v>
       </c>
       <c r="B364">
-        <v>42.75</v>
+        <v>32.625</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3286,7 +3286,7 @@
         <v>363</v>
       </c>
       <c r="B365">
-        <v>33.75</v>
+        <v>30.2416666666666</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3294,7 +3294,7 @@
         <v>364</v>
       </c>
       <c r="B366">
-        <v>27</v>
+        <v>29.5201754385964</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3302,7 +3302,7 @@
         <v>365</v>
       </c>
       <c r="B367">
-        <v>29.725</v>
+        <v>38.25</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -3310,7 +3310,7 @@
         <v>366</v>
       </c>
       <c r="B368">
-        <v>26.55</v>
+        <v>38.125</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -3318,7 +3318,7 @@
         <v>367</v>
       </c>
       <c r="B369">
-        <v>23.6666666666666</v>
+        <v>45.125</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -3326,7 +3326,7 @@
         <v>368</v>
       </c>
       <c r="B370">
-        <v>17.7670454545454</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -3334,7 +3334,7 @@
         <v>369</v>
       </c>
       <c r="B371">
-        <v>19.5</v>
+        <v>26.875</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -3342,7 +3342,7 @@
         <v>370</v>
       </c>
       <c r="B372">
-        <v>21.0961538461538</v>
+        <v>25.125</v>
       </c>
     </row>
     <row r="373" spans="1:2">
@@ -3350,7 +3350,7 @@
         <v>371</v>
       </c>
       <c r="B373">
-        <v>26.5666666666666</v>
+        <v>31.125</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -3358,7 +3358,7 @@
         <v>372</v>
       </c>
       <c r="B374">
-        <v>15.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -3366,7 +3366,7 @@
         <v>373</v>
       </c>
       <c r="B375">
-        <v>47.375</v>
+        <v>21.625</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -3374,7 +3374,7 @@
         <v>374</v>
       </c>
       <c r="B376">
-        <v>66.125</v>
+        <v>17</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -3382,7 +3382,7 @@
         <v>375</v>
       </c>
       <c r="B377">
-        <v>18.525</v>
+        <v>22.2916666666666</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -3390,7 +3390,7 @@
         <v>376</v>
       </c>
       <c r="B378">
-        <v>13.1333333333333</v>
+        <v>20.875</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -3398,7 +3398,7 @@
         <v>377</v>
       </c>
       <c r="B379">
-        <v>17.75</v>
+        <v>10.1916666666666</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -3406,7 +3406,7 @@
         <v>378</v>
       </c>
       <c r="B380">
-        <v>21.75</v>
+        <v>15.35</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -3414,7 +3414,7 @@
         <v>379</v>
       </c>
       <c r="B381">
-        <v>34</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -3422,7 +3422,7 @@
         <v>380</v>
       </c>
       <c r="B382">
-        <v>13.75</v>
+        <v>7.625</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -3430,7 +3430,7 @@
         <v>381</v>
       </c>
       <c r="B383">
-        <v>3.2</v>
+        <v>20.375</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -3438,7 +3438,7 @@
         <v>382</v>
       </c>
       <c r="B384">
-        <v>13.3875</v>
+        <v>23.7972222222222</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -3446,7 +3446,7 @@
         <v>383</v>
       </c>
       <c r="B385">
-        <v>10.5</v>
+        <v>39.375</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -3454,7 +3454,7 @@
         <v>384</v>
       </c>
       <c r="B386">
-        <v>20.75</v>
+        <v>15.7416666666666</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -3462,7 +3462,7 @@
         <v>385</v>
       </c>
       <c r="B387">
-        <v>12</v>
+        <v>45.3833333333333</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -3470,7 +3470,7 @@
         <v>386</v>
       </c>
       <c r="B388">
-        <v>7.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -3478,7 +3478,7 @@
         <v>387</v>
       </c>
       <c r="B389">
-        <v>20.5</v>
+        <v>32.875</v>
       </c>
     </row>
     <row r="390" spans="1:2">
@@ -3486,7 +3486,7 @@
         <v>388</v>
       </c>
       <c r="B390">
-        <v>12</v>
+        <v>31.8666666666666</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -3494,7 +3494,7 @@
         <v>389</v>
       </c>
       <c r="B391">
-        <v>23.7972222222222</v>
+        <v>35.7583333333333</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -3502,7 +3502,7 @@
         <v>390</v>
       </c>
       <c r="B392">
-        <v>20.375</v>
+        <v>28</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -3510,7 +3510,7 @@
         <v>391</v>
       </c>
       <c r="B393">
-        <v>26.3166666666666</v>
+        <v>23.0833333333333</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -3518,7 +3518,7 @@
         <v>392</v>
       </c>
       <c r="B394">
-        <v>37.1333333333333</v>
+        <v>22.6583333333333</v>
       </c>
     </row>
     <row r="395" spans="1:2">
@@ -3526,7 +3526,7 @@
         <v>393</v>
       </c>
       <c r="B395">
-        <v>32.7115384615384</v>
+        <v>12.1875</v>
       </c>
     </row>
     <row r="396" spans="1:2">
@@ -3534,7 +3534,7 @@
         <v>394</v>
       </c>
       <c r="B396">
-        <v>34.75</v>
+        <v>30.2833333333333</v>
       </c>
     </row>
     <row r="397" spans="1:2">
@@ -3542,7 +3542,7 @@
         <v>395</v>
       </c>
       <c r="B397">
-        <v>38.125</v>
+        <v>38.375</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -3550,7 +3550,7 @@
         <v>396</v>
       </c>
       <c r="B398">
-        <v>27.6363636363636</v>
+        <v>47.375</v>
       </c>
     </row>
     <row r="399" spans="1:2">
@@ -3558,7 +3558,7 @@
         <v>397</v>
       </c>
       <c r="B399">
-        <v>32.625</v>
+        <v>25.1346153846153</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -3566,7 +3566,7 @@
         <v>398</v>
       </c>
       <c r="B400">
-        <v>41.75</v>
+        <v>23.625</v>
       </c>
     </row>
     <row r="401" spans="1:2">
@@ -3574,7 +3574,7 @@
         <v>399</v>
       </c>
       <c r="B401">
-        <v>41.375</v>
+        <v>28.125</v>
       </c>
     </row>
     <row r="402" spans="1:2">
@@ -3582,7 +3582,7 @@
         <v>400</v>
       </c>
       <c r="B402">
-        <v>9.39824561403508</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="403" spans="1:2">
@@ -3590,7 +3590,7 @@
         <v>401</v>
       </c>
       <c r="B403">
-        <v>9.65384615384615</v>
+        <v>25.125</v>
       </c>
     </row>
     <row r="404" spans="1:2">
@@ -3598,7 +3598,7 @@
         <v>402</v>
       </c>
       <c r="B404">
-        <v>33.5166666666666</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="405" spans="1:2">
@@ -3606,7 +3606,7 @@
         <v>403</v>
       </c>
       <c r="B405">
-        <v>32.1416666666666</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="406" spans="1:2">
@@ -3614,7 +3614,7 @@
         <v>404</v>
       </c>
       <c r="B406">
-        <v>29.25</v>
+        <v>10.7083333333333</v>
       </c>
     </row>
     <row r="407" spans="1:2">
@@ -3622,7 +3622,7 @@
         <v>405</v>
       </c>
       <c r="B407">
-        <v>30.875</v>
+        <v>8.63461538461538</v>
       </c>
     </row>
     <row r="408" spans="1:2">
@@ -3630,7 +3630,7 @@
         <v>406</v>
       </c>
       <c r="B408">
-        <v>33.25</v>
+        <v>16.1666666666666</v>
       </c>
     </row>
     <row r="409" spans="1:2">
@@ -3638,7 +3638,7 @@
         <v>407</v>
       </c>
       <c r="B409">
-        <v>28.25</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="410" spans="1:2">
@@ -3646,7 +3646,7 @@
         <v>408</v>
       </c>
       <c r="B410">
-        <v>39.2333333333333</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="411" spans="1:2">
@@ -3654,7 +3654,7 @@
         <v>409</v>
       </c>
       <c r="B411">
-        <v>28.5916666666666</v>
+        <v>34.75</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -3662,7 +3662,7 @@
         <v>410</v>
       </c>
       <c r="B412">
-        <v>29.625</v>
+        <v>39.6333333333333</v>
       </c>
     </row>
     <row r="413" spans="1:2">
@@ -3670,7 +3670,7 @@
         <v>411</v>
       </c>
       <c r="B413">
-        <v>30.2833333333333</v>
+        <v>32.6333333333333</v>
       </c>
     </row>
     <row r="414" spans="1:2">
@@ -3678,7 +3678,7 @@
         <v>412</v>
       </c>
       <c r="B414">
-        <v>24.7</v>
+        <v>22.45</v>
       </c>
     </row>
     <row r="415" spans="1:2">
@@ -3686,7 +3686,7 @@
         <v>413</v>
       </c>
       <c r="B415">
-        <v>9.098214285714279</v>
+        <v>33.2916666666666</v>
       </c>
     </row>
     <row r="416" spans="1:2">
@@ -3694,7 +3694,7 @@
         <v>414</v>
       </c>
       <c r="B416">
-        <v>9.58333333333333</v>
+        <v>37.25</v>
       </c>
     </row>
     <row r="417" spans="1:2">
@@ -3702,7 +3702,7 @@
         <v>415</v>
       </c>
       <c r="B417">
-        <v>15.5</v>
+        <v>37.625</v>
       </c>
     </row>
     <row r="418" spans="1:2">
@@ -3710,7 +3710,7 @@
         <v>416</v>
       </c>
       <c r="B418">
-        <v>22.8898809523809</v>
+        <v>25.2656862745098</v>
       </c>
     </row>
     <row r="419" spans="1:2">
@@ -3718,7 +3718,7 @@
         <v>417</v>
       </c>
       <c r="B419">
-        <v>68.125</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="420" spans="1:2">
@@ -3726,7 +3726,7 @@
         <v>418</v>
       </c>
       <c r="B420">
-        <v>63.475</v>
+        <v>29.7083333333333</v>
       </c>
     </row>
     <row r="421" spans="1:2">
@@ -3734,7 +3734,7 @@
         <v>419</v>
       </c>
       <c r="B421">
-        <v>25.1346153846153</v>
+        <v>33.275</v>
       </c>
     </row>
     <row r="422" spans="1:2">
@@ -3742,7 +3742,7 @@
         <v>420</v>
       </c>
       <c r="B422">
-        <v>25.125</v>
+        <v>32.5384615384615</v>
       </c>
     </row>
     <row r="423" spans="1:2">
@@ -3750,7 +3750,7 @@
         <v>421</v>
       </c>
       <c r="B423">
-        <v>28.125</v>
+        <v>31.5166666666666</v>
       </c>
     </row>
     <row r="424" spans="1:2">
@@ -3758,7 +3758,7 @@
         <v>422</v>
       </c>
       <c r="B424">
-        <v>19.0166666666666</v>
+        <v>30.75</v>
       </c>
     </row>
     <row r="425" spans="1:2">
@@ -3766,7 +3766,7 @@
         <v>423</v>
       </c>
       <c r="B425">
-        <v>18.625</v>
+        <v>34.3055555555555</v>
       </c>
     </row>
     <row r="426" spans="1:2">
@@ -3774,7 +3774,7 @@
         <v>424</v>
       </c>
       <c r="B426">
-        <v>39.5916666666666</v>
+        <v>21.8203125</v>
       </c>
     </row>
     <row r="427" spans="1:2">
@@ -3782,7 +3782,7 @@
         <v>425</v>
       </c>
       <c r="B427">
-        <v>62.375</v>
+        <v>36.8916666666666</v>
       </c>
     </row>
     <row r="428" spans="1:2">
@@ -3790,7 +3790,7 @@
         <v>426</v>
       </c>
       <c r="B428">
-        <v>45.3833333333333</v>
+        <v>41.8583333333333</v>
       </c>
     </row>
     <row r="429" spans="1:2">
@@ -3798,7 +3798,7 @@
         <v>427</v>
       </c>
       <c r="B429">
-        <v>76.52500000000001</v>
+        <v>12.93125</v>
       </c>
     </row>
     <row r="430" spans="1:2">
@@ -3806,7 +3806,7 @@
         <v>428</v>
       </c>
       <c r="B430">
-        <v>42.8666666666666</v>
+        <v>9.09848484848485</v>
       </c>
     </row>
     <row r="431" spans="1:2">
@@ -3814,7 +3814,7 @@
         <v>429</v>
       </c>
       <c r="B431">
-        <v>43.6166666666666</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="432" spans="1:2">
@@ -3822,7 +3822,7 @@
         <v>430</v>
       </c>
       <c r="B432">
-        <v>42.5</v>
+        <v>18.0486111111111</v>
       </c>
     </row>
     <row r="433" spans="1:2">
@@ -3830,7 +3830,7 @@
         <v>431</v>
       </c>
       <c r="B433">
-        <v>51.7561111111111</v>
+        <v>31.8839285714285</v>
       </c>
     </row>
     <row r="434" spans="1:2">
@@ -3838,7 +3838,7 @@
         <v>432</v>
       </c>
       <c r="B434">
-        <v>52.25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="435" spans="1:2">
@@ -3846,7 +3846,7 @@
         <v>433</v>
       </c>
       <c r="B435">
-        <v>47.9333333333333</v>
+        <v>46.4916666666666</v>
       </c>
     </row>
     <row r="436" spans="1:2">
@@ -3854,7 +3854,7 @@
         <v>434</v>
       </c>
       <c r="B436">
-        <v>9.33522727272727</v>
+        <v>15.7222222222222</v>
       </c>
     </row>
     <row r="437" spans="1:2">
@@ -3862,7 +3862,7 @@
         <v>435</v>
       </c>
       <c r="B437">
-        <v>37.9333333333333</v>
+        <v>8.93928571428571</v>
       </c>
     </row>
     <row r="438" spans="1:2">
@@ -3870,7 +3870,7 @@
         <v>436</v>
       </c>
       <c r="B438">
-        <v>35.7583333333333</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="439" spans="1:2">
@@ -3878,7 +3878,7 @@
         <v>437</v>
       </c>
       <c r="B439">
-        <v>28</v>
+        <v>16.765625</v>
       </c>
     </row>
     <row r="440" spans="1:2">
@@ -3886,7 +3886,7 @@
         <v>438</v>
       </c>
       <c r="B440">
-        <v>15.9916666666666</v>
+        <v>20.75</v>
       </c>
     </row>
     <row r="441" spans="1:2">
@@ -3894,7 +3894,7 @@
         <v>439</v>
       </c>
       <c r="B441">
-        <v>10.875</v>
+        <v>13.8833333333333</v>
       </c>
     </row>
     <row r="442" spans="1:2">
@@ -3902,7 +3902,7 @@
         <v>440</v>
       </c>
       <c r="B442">
-        <v>13.75</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="443" spans="1:2">
@@ -3910,7 +3910,7 @@
         <v>441</v>
       </c>
       <c r="B443">
-        <v>11.4</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="444" spans="1:2">
@@ -3918,7 +3918,7 @@
         <v>442</v>
       </c>
       <c r="B444">
-        <v>5.7578125</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="445" spans="1:2">
@@ -3926,7 +3926,7 @@
         <v>443</v>
       </c>
       <c r="B445">
-        <v>9.46875</v>
+        <v>5.32142857142857</v>
       </c>
     </row>
     <row r="446" spans="1:2">
@@ -3934,7 +3934,7 @@
         <v>444</v>
       </c>
       <c r="B446">
-        <v>14.625</v>
+        <v>42.025</v>
       </c>
     </row>
     <row r="447" spans="1:2">
@@ -3942,7 +3942,7 @@
         <v>445</v>
       </c>
       <c r="B447">
-        <v>16.5416666666666</v>
+        <v>9.29166666666666</v>
       </c>
     </row>
     <row r="448" spans="1:2">
@@ -3950,7 +3950,7 @@
         <v>446</v>
       </c>
       <c r="B448">
-        <v>15.125</v>
+        <v>21.9464285714285</v>
       </c>
     </row>
     <row r="449" spans="1:2">
@@ -3958,7 +3958,7 @@
         <v>447</v>
       </c>
       <c r="B449">
-        <v>38.5</v>
+        <v>12.4333333333333</v>
       </c>
     </row>
     <row r="450" spans="1:2">
@@ -3966,7 +3966,7 @@
         <v>448</v>
       </c>
       <c r="B450">
-        <v>34.5833333333333</v>
+        <v>15.6590909090909</v>
       </c>
     </row>
     <row r="451" spans="1:2">
@@ -3974,7 +3974,7 @@
         <v>449</v>
       </c>
       <c r="B451">
-        <v>32.4610795454545</v>
+        <v>10.640625</v>
       </c>
     </row>
     <row r="452" spans="1:2">
@@ -3982,7 +3982,7 @@
         <v>450</v>
       </c>
       <c r="B452">
-        <v>38.6666666666666</v>
+        <v>16.075</v>
       </c>
     </row>
     <row r="453" spans="1:2">
@@ -3990,7 +3990,7 @@
         <v>451</v>
       </c>
       <c r="B453">
-        <v>32.375</v>
+        <v>14.2293233082706</v>
       </c>
     </row>
     <row r="454" spans="1:2">
@@ -3998,7 +3998,7 @@
         <v>452</v>
       </c>
       <c r="B454">
-        <v>32.2166666666666</v>
+        <v>23.4722222222222</v>
       </c>
     </row>
     <row r="455" spans="1:2">
@@ -4006,7 +4006,7 @@
         <v>453</v>
       </c>
       <c r="B455">
-        <v>32.65</v>
+        <v>14.8875</v>
       </c>
     </row>
     <row r="456" spans="1:2">
@@ -4014,7 +4014,7 @@
         <v>454</v>
       </c>
       <c r="B456">
-        <v>19.1052631578947</v>
+        <v>28.125</v>
       </c>
     </row>
     <row r="457" spans="1:2">
@@ -4022,7 +4022,7 @@
         <v>455</v>
       </c>
       <c r="B457">
-        <v>30.75</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="458" spans="1:2">
@@ -4030,7 +4030,7 @@
         <v>456</v>
       </c>
       <c r="B458">
-        <v>34.3055555555555</v>
+        <v>23.5916666666666</v>
       </c>
     </row>
     <row r="459" spans="1:2">
@@ -4038,7 +4038,7 @@
         <v>457</v>
       </c>
       <c r="B459">
-        <v>18.0486111111111</v>
+        <v>15.7894736842105</v>
       </c>
     </row>
     <row r="460" spans="1:2">
@@ -4046,7 +4046,7 @@
         <v>458</v>
       </c>
       <c r="B460">
-        <v>16.2166666666666</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="461" spans="1:2">
@@ -4054,7 +4054,7 @@
         <v>459</v>
       </c>
       <c r="B461">
-        <v>18.65</v>
+        <v>5.1875</v>
       </c>
     </row>
     <row r="462" spans="1:2">
@@ -4062,7 +4062,7 @@
         <v>460</v>
       </c>
       <c r="B462">
-        <v>11.1309523809523</v>
+        <v>26.7965116279069</v>
       </c>
     </row>
     <row r="463" spans="1:2">
@@ -4070,7 +4070,7 @@
         <v>461</v>
       </c>
       <c r="B463">
-        <v>7.875</v>
+        <v>24.4958333333333</v>
       </c>
     </row>
     <row r="464" spans="1:2">
@@ -4078,7 +4078,7 @@
         <v>462</v>
       </c>
       <c r="B464">
-        <v>18.325</v>
+        <v>11.6375</v>
       </c>
     </row>
     <row r="465" spans="1:2">
@@ -4086,7 +4086,7 @@
         <v>463</v>
       </c>
       <c r="B465">
-        <v>13.3888888888888</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="466" spans="1:2">
@@ -4094,7 +4094,7 @@
         <v>464</v>
       </c>
       <c r="B466">
-        <v>17.625</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="467" spans="1:2">
@@ -4102,7 +4102,7 @@
         <v>465</v>
       </c>
       <c r="B467">
-        <v>51.75</v>
+        <v>42.8666666666666</v>
       </c>
     </row>
     <row r="468" spans="1:2">
@@ -4110,7 +4110,7 @@
         <v>466</v>
       </c>
       <c r="B468">
-        <v>100</v>
+        <v>43.6166666666666</v>
       </c>
     </row>
     <row r="469" spans="1:2">
@@ -4118,7 +4118,7 @@
         <v>467</v>
       </c>
       <c r="B469">
-        <v>7.53125</v>
+        <v>29.725</v>
       </c>
     </row>
     <row r="470" spans="1:2">
@@ -4126,7 +4126,7 @@
         <v>468</v>
       </c>
       <c r="B470">
-        <v>25.25</v>
+        <v>26.55</v>
       </c>
     </row>
     <row r="471" spans="1:2">
@@ -4134,7 +4134,7 @@
         <v>469</v>
       </c>
       <c r="B471">
-        <v>52.25</v>
+        <v>23.6666666666666</v>
       </c>
     </row>
     <row r="472" spans="1:2">
@@ -4142,7 +4142,7 @@
         <v>470</v>
       </c>
       <c r="B472">
-        <v>21.9464285714285</v>
+        <v>15.7833333333333</v>
       </c>
     </row>
     <row r="473" spans="1:2">
@@ -4150,7 +4150,7 @@
         <v>471</v>
       </c>
       <c r="B473">
-        <v>12.4333333333333</v>
+        <v>17.7670454545454</v>
       </c>
     </row>
     <row r="474" spans="1:2">
@@ -4158,7 +4158,7 @@
         <v>472</v>
       </c>
       <c r="B474">
-        <v>9.291666666666661</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="475" spans="1:2">
@@ -4166,7 +4166,7 @@
         <v>473</v>
       </c>
       <c r="B475">
-        <v>16.25</v>
+        <v>17.9375</v>
       </c>
     </row>
     <row r="476" spans="1:2">
@@ -4174,7 +4174,7 @@
         <v>474</v>
       </c>
       <c r="B476">
-        <v>8.75</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="477" spans="1:2">
@@ -4182,7 +4182,7 @@
         <v>475</v>
       </c>
       <c r="B477">
-        <v>10.25</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="478" spans="1:2">
@@ -4190,7 +4190,7 @@
         <v>476</v>
       </c>
       <c r="B478">
-        <v>7.65833333333333</v>
+        <v>18.65</v>
       </c>
     </row>
     <row r="479" spans="1:2">
@@ -4198,7 +4198,7 @@
         <v>477</v>
       </c>
       <c r="B479">
-        <v>25.125</v>
+        <v>26.625</v>
       </c>
     </row>
     <row r="480" spans="1:2">
@@ -4206,7 +4206,7 @@
         <v>478</v>
       </c>
       <c r="B480">
-        <v>14.75</v>
+        <v>10.8083333333333</v>
       </c>
     </row>
     <row r="481" spans="1:2">
@@ -4214,7 +4214,7 @@
         <v>479</v>
       </c>
       <c r="B481">
-        <v>23.5</v>
+        <v>22.375</v>
       </c>
     </row>
     <row r="482" spans="1:2">
@@ -4222,7 +4222,7 @@
         <v>480</v>
       </c>
       <c r="B482">
-        <v>23.575</v>
+        <v>28.5916666666666</v>
       </c>
     </row>
     <row r="483" spans="1:2">
@@ -4230,7 +4230,7 @@
         <v>481</v>
       </c>
       <c r="B483">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="484" spans="1:2">
@@ -4238,7 +4238,7 @@
         <v>482</v>
       </c>
       <c r="B484">
-        <v>17.8916666666666</v>
+        <v>32.1346153846153</v>
       </c>
     </row>
     <row r="485" spans="1:2">
@@ -4246,7 +4246,7 @@
         <v>483</v>
       </c>
       <c r="B485">
-        <v>13.3571428571428</v>
+        <v>53.875</v>
       </c>
     </row>
     <row r="486" spans="1:2">
@@ -4254,7 +4254,7 @@
         <v>484</v>
       </c>
       <c r="B486">
-        <v>20</v>
+        <v>52.7083333333333</v>
       </c>
     </row>
     <row r="487" spans="1:2">
@@ -4262,7 +4262,7 @@
         <v>485</v>
       </c>
       <c r="B487">
-        <v>24.05</v>
+        <v>26.7954545454545</v>
       </c>
     </row>
     <row r="488" spans="1:2">
@@ -4270,7 +4270,7 @@
         <v>486</v>
       </c>
       <c r="B488">
-        <v>24.125</v>
+        <v>24.7916666666666</v>
       </c>
     </row>
     <row r="489" spans="1:2">
@@ -4278,7 +4278,7 @@
         <v>487</v>
       </c>
       <c r="B489">
-        <v>13.725</v>
+        <v>29.875</v>
       </c>
     </row>
     <row r="490" spans="1:2">
@@ -4286,7 +4286,7 @@
         <v>488</v>
       </c>
       <c r="B490">
-        <v>18.125</v>
+        <v>27.9666666666666</v>
       </c>
     </row>
     <row r="491" spans="1:2">
@@ -4294,7 +4294,7 @@
         <v>489</v>
       </c>
       <c r="B491">
-        <v>15.1916666666666</v>
+        <v>52.25</v>
       </c>
     </row>
     <row r="492" spans="1:2">
@@ -4302,7 +4302,7 @@
         <v>490</v>
       </c>
       <c r="B492">
-        <v>19.875</v>
+        <v>37.0416666666666</v>
       </c>
     </row>
     <row r="493" spans="1:2">
@@ -4310,7 +4310,7 @@
         <v>491</v>
       </c>
       <c r="B493">
-        <v>23.35</v>
+        <v>33.3214285714285</v>
       </c>
     </row>
     <row r="494" spans="1:2">
@@ -4318,7 +4318,7 @@
         <v>492</v>
       </c>
       <c r="B494">
-        <v>11.6339285714285</v>
+        <v>19.4145833333333</v>
       </c>
     </row>
     <row r="495" spans="1:2">
@@ -4326,7 +4326,7 @@
         <v>493</v>
       </c>
       <c r="B495">
-        <v>22.25</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="496" spans="1:2">
@@ -4334,7 +4334,7 @@
         <v>494</v>
       </c>
       <c r="B496">
-        <v>13.9772727272727</v>
+        <v>18.325</v>
       </c>
     </row>
     <row r="497" spans="1:2">
@@ -4342,7 +4342,7 @@
         <v>495</v>
       </c>
       <c r="B497">
-        <v>6.89583333333333</v>
+        <v>17.625</v>
       </c>
     </row>
     <row r="498" spans="1:2">
@@ -4350,7 +4350,7 @@
         <v>496</v>
       </c>
       <c r="B498">
-        <v>21.6538461538461</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="499" spans="1:2">
@@ -4358,7 +4358,7 @@
         <v>497</v>
       </c>
       <c r="B499">
-        <v>18.125</v>
+        <v>12</v>
       </c>
     </row>
     <row r="500" spans="1:2">
@@ -4366,7 +4366,7 @@
         <v>498</v>
       </c>
       <c r="B500">
-        <v>3.84821428571428</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="501" spans="1:2">
@@ -4374,7 +4374,7 @@
         <v>499</v>
       </c>
       <c r="B501">
-        <v>33.5</v>
+        <v>19.625</v>
       </c>
     </row>
     <row r="502" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>500</v>
       </c>
       <c r="B502">
-        <v>11</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="503" spans="1:2">
@@ -4390,7 +4390,7 @@
         <v>501</v>
       </c>
       <c r="B503">
-        <v>20.875</v>
+        <v>42.75</v>
       </c>
     </row>
     <row r="504" spans="1:2">
@@ -4398,7 +4398,7 @@
         <v>502</v>
       </c>
       <c r="B504">
-        <v>21.625</v>
+        <v>38.125</v>
       </c>
     </row>
     <row r="505" spans="1:2">
@@ -4406,7 +4406,7 @@
         <v>503</v>
       </c>
       <c r="B505">
-        <v>17</v>
+        <v>41.625</v>
       </c>
     </row>
     <row r="506" spans="1:2">
@@ -4414,7 +4414,7 @@
         <v>504</v>
       </c>
       <c r="B506">
-        <v>22.2916666666666</v>
+        <v>34</v>
       </c>
     </row>
     <row r="507" spans="1:2">
@@ -4422,7 +4422,7 @@
         <v>505</v>
       </c>
       <c r="B507">
-        <v>10.1916666666666</v>
+        <v>5.925</v>
       </c>
     </row>
     <row r="508" spans="1:2">
@@ -4430,7 +4430,7 @@
         <v>506</v>
       </c>
       <c r="B508">
-        <v>15.35</v>
+        <v>8.09523809523809</v>
       </c>
     </row>
     <row r="509" spans="1:2">
@@ -4438,7 +4438,7 @@
         <v>507</v>
       </c>
       <c r="B509">
-        <v>12.7</v>
+        <v>13.1333333333333</v>
       </c>
     </row>
     <row r="510" spans="1:2">
@@ -4446,7 +4446,7 @@
         <v>508</v>
       </c>
       <c r="B510">
-        <v>19.4145833333333</v>
+        <v>3.00098039215686</v>
       </c>
     </row>
     <row r="511" spans="1:2">
@@ -4454,7 +4454,7 @@
         <v>509</v>
       </c>
       <c r="B511">
-        <v>7.14583333333333</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="512" spans="1:2">
@@ -4462,7 +4462,7 @@
         <v>510</v>
       </c>
       <c r="B512">
-        <v>16.875</v>
+        <v>18.125</v>
       </c>
     </row>
     <row r="513" spans="1:2">
@@ -4470,7 +4470,7 @@
         <v>511</v>
       </c>
       <c r="B513">
-        <v>6.03571428571428</v>
+        <v>13.725</v>
       </c>
     </row>
     <row r="514" spans="1:2">
@@ -4478,7 +4478,7 @@
         <v>512</v>
       </c>
       <c r="B514">
-        <v>8.801960784313721</v>
+        <v>57.125</v>
       </c>
     </row>
     <row r="515" spans="1:2">
@@ -4486,7 +4486,7 @@
         <v>513</v>
       </c>
       <c r="B515">
-        <v>6</v>
+        <v>85.625</v>
       </c>
     </row>
     <row r="516" spans="1:2">
@@ -4494,7 +4494,7 @@
         <v>514</v>
       </c>
       <c r="B516">
-        <v>10.3839285714285</v>
+        <v>45.625</v>
       </c>
     </row>
     <row r="517" spans="1:2">
@@ -4502,7 +4502,7 @@
         <v>515</v>
       </c>
       <c r="B517">
-        <v>10.4652777777777</v>
+        <v>15.6538461538461</v>
       </c>
     </row>
     <row r="518" spans="1:2">
@@ -4510,7 +4510,7 @@
         <v>516</v>
       </c>
       <c r="B518">
-        <v>8.79761904761904</v>
+        <v>9.65625</v>
       </c>
     </row>
     <row r="519" spans="1:2">
@@ -4518,7 +4518,7 @@
         <v>517</v>
       </c>
       <c r="B519">
-        <v>15.7222222222222</v>
+        <v>15.15</v>
       </c>
     </row>
     <row r="520" spans="1:2">
@@ -4526,7 +4526,7 @@
         <v>518</v>
       </c>
       <c r="B520">
-        <v>8.09523809523809</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="521" spans="1:2">
@@ -4534,7 +4534,7 @@
         <v>519</v>
       </c>
       <c r="B521">
-        <v>3.00098039215686</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="522" spans="1:2">
@@ -4542,7 +4542,7 @@
         <v>520</v>
       </c>
       <c r="B522">
-        <v>5.925</v>
+        <v>18.0833333333333</v>
       </c>
     </row>
     <row r="523" spans="1:2">
@@ -4550,7 +4550,7 @@
         <v>521</v>
       </c>
       <c r="B523">
-        <v>48.05</v>
+        <v>26.1333333333333</v>
       </c>
     </row>
     <row r="524" spans="1:2">
@@ -4558,7 +4558,7 @@
         <v>522</v>
       </c>
       <c r="B524">
-        <v>11.375</v>
+        <v>23.8926470588235</v>
       </c>
     </row>
     <row r="525" spans="1:2">
@@ -4566,7 +4566,7 @@
         <v>523</v>
       </c>
       <c r="B525">
-        <v>34.5</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="526" spans="1:2">
@@ -4574,7 +4574,7 @@
         <v>524</v>
       </c>
       <c r="B526">
-        <v>27</v>
+        <v>69.625</v>
       </c>
     </row>
     <row r="527" spans="1:2">
@@ -4582,7 +4582,7 @@
         <v>525</v>
       </c>
       <c r="B527">
-        <v>26.875</v>
+        <v>37.25</v>
       </c>
     </row>
     <row r="528" spans="1:2">
@@ -4590,7 +4590,7 @@
         <v>526</v>
       </c>
       <c r="B528">
-        <v>5.32142857142857</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="529" spans="1:2">
@@ -4598,7 +4598,7 @@
         <v>527</v>
       </c>
       <c r="B529">
-        <v>5.25</v>
+        <v>27.875</v>
       </c>
     </row>
     <row r="530" spans="1:2">
@@ -4606,7 +4606,7 @@
         <v>528</v>
       </c>
       <c r="B530">
-        <v>3.00681818181818</v>
+        <v>28.45</v>
       </c>
     </row>
     <row r="531" spans="1:2">
@@ -4614,7 +4614,7 @@
         <v>529</v>
       </c>
       <c r="B531">
-        <v>10.25</v>
+        <v>2.6328125</v>
       </c>
     </row>
     <row r="532" spans="1:2">
@@ -4622,7 +4622,7 @@
         <v>530</v>
       </c>
       <c r="B532">
-        <v>6.875</v>
+        <v>15.2458333333333</v>
       </c>
     </row>
     <row r="533" spans="1:2">
@@ -4630,7 +4630,7 @@
         <v>531</v>
       </c>
       <c r="B533">
-        <v>6.63194444444444</v>
+        <v>26.3166666666666</v>
       </c>
     </row>
     <row r="534" spans="1:2">
@@ -4638,7 +4638,7 @@
         <v>532</v>
       </c>
       <c r="B534">
-        <v>13.2083333333333</v>
+        <v>5.90384615384615</v>
       </c>
     </row>
     <row r="535" spans="1:2">
@@ -4646,7 +4646,7 @@
         <v>533</v>
       </c>
       <c r="B535">
-        <v>12.675</v>
+        <v>13.865</v>
       </c>
     </row>
     <row r="536" spans="1:2">
@@ -4654,7 +4654,7 @@
         <v>534</v>
       </c>
       <c r="B536">
-        <v>12.25</v>
+        <v>9.28571428571428</v>
       </c>
     </row>
     <row r="537" spans="1:2">
@@ -4662,7 +4662,7 @@
         <v>535</v>
       </c>
       <c r="B537">
-        <v>35.2666666666666</v>
+        <v>19.1052631578947</v>
       </c>
     </row>
     <row r="538" spans="1:2">
@@ -4670,7 +4670,7 @@
         <v>536</v>
       </c>
       <c r="B538">
-        <v>41.8583333333333</v>
+        <v>14.7397435897435</v>
       </c>
     </row>
     <row r="539" spans="1:2">
@@ -4678,7 +4678,7 @@
         <v>537</v>
       </c>
       <c r="B539">
-        <v>13.865</v>
+        <v>9.39824561403508</v>
       </c>
     </row>
     <row r="540" spans="1:2">
@@ -4686,7 +4686,7 @@
         <v>538</v>
       </c>
       <c r="B540">
-        <v>9.285714285714279</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="541" spans="1:2">
@@ -4694,7 +4694,39 @@
         <v>539</v>
       </c>
       <c r="B541">
+        <v>9.65384615384615</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2">
+      <c r="A542" s="1">
+        <v>540</v>
+      </c>
+      <c r="B542">
         <v>11.0833333333333</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2">
+      <c r="A543" s="1">
+        <v>541</v>
+      </c>
+      <c r="B543">
+        <v>32.625</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2">
+      <c r="A544" s="1">
+        <v>542</v>
+      </c>
+      <c r="B544">
+        <v>26.9166666666666</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2">
+      <c r="A545" s="1">
+        <v>543</v>
+      </c>
+      <c r="B545">
+        <v>26.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>